<commit_message>
Depreciation calculator and analysis files
</commit_message>
<xml_diff>
--- a/Project-1(Depreciation-Calculator-Excel).xlsx
+++ b/Project-1(Depreciation-Calculator-Excel).xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMBIKA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMBIKA\Desktop\Coachx.Live\Submitted Work\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DBE806-3058-482A-BFF3-925BD210ACE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F52A213-A958-44B3-8C13-A97CE87E7557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Information" sheetId="2" r:id="rId1"/>
-    <sheet name="Depreciation Calculator" sheetId="1" r:id="rId2"/>
+    <sheet name="Depreciation Calculator" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -368,34 +367,34 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -417,296 +416,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1581150" y="219075"/>
-          <a:ext cx="14516100" cy="733425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>     </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="3200" b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Comparative Analysis of Depreciation Methods: Straight-Line vs. Diminishing Balance</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1533525" y="1390650"/>
-          <a:ext cx="14754225" cy="5619750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000">
-            <a:solidFill>
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" i="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Point</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>s to remember before starting this project:-</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="2000">
-            <a:solidFill>
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Purpose of the project is to give you the fundamental ideas about how Depreciation methods  and terminologies works in Excel so imp thing is to go thorough this documentation very carefully and understand the tems.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="2000">
-            <a:solidFill>
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>1. In Project Worksheets you dataset is already prepared  so you have to find the values and answers for given functions for solution please go through this sheet </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="2000">
-            <a:solidFill>
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>2. Kindly read all the documentation attached to this project file very carefully because all the important points for making this projects is given there in this documentation</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="2000">
-            <a:solidFill>
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>3. After doing the anlalysis Create a Summary report that what insights and analysis you have find while doing this proects</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="2000">
-            <a:solidFill>
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1117,24 +826,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
@@ -1163,20 +854,20 @@
     </row>
     <row r="2" spans="1:5" ht="37.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" ht="25.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1188,19 +879,19 @@
     </row>
     <row r="5" spans="1:5" ht="25.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="10">
         <v>450000</v>
       </c>
@@ -1208,10 +899,10 @@
     </row>
     <row r="7" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="10">
         <v>50000</v>
       </c>
@@ -1219,10 +910,10 @@
     </row>
     <row r="8" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="4">
         <f>D6+D7</f>
         <v>500000</v>
@@ -1231,10 +922,10 @@
     </row>
     <row r="9" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="10">
         <v>50000</v>
       </c>
@@ -1242,10 +933,10 @@
     </row>
     <row r="10" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="11">
         <v>10</v>
       </c>
@@ -1253,10 +944,10 @@
     </row>
     <row r="11" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="4">
         <f>IF(D8="", "", SLN($D$8,$D$9,$D$10))</f>
         <v>45000</v>
@@ -1265,10 +956,10 @@
     </row>
     <row r="12" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="6">
         <f>IFERROR(D11/D8,"")</f>
         <v>0.09</v>
@@ -1277,10 +968,10 @@
     </row>
     <row r="13" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="3">
         <f>IF(D8="", "", D11*D10)</f>
         <v>450000</v>
@@ -1289,10 +980,10 @@
     </row>
     <row r="14" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="3">
         <f>IF(D8="", "", D8-D13)</f>
         <v>50000</v>
@@ -1301,10 +992,10 @@
     </row>
     <row r="15" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="3">
         <f>IF(D8="", "", D9-D14)</f>
         <v>0</v>
@@ -1320,19 +1011,19 @@
     </row>
     <row r="17" spans="1:5" ht="25.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="10">
         <v>450000</v>
       </c>
@@ -1340,10 +1031,10 @@
     </row>
     <row r="19" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="14"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="10">
         <v>50000</v>
       </c>
@@ -1351,10 +1042,10 @@
     </row>
     <row r="20" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="4">
         <f>+D18+D19</f>
         <v>500000</v>
@@ -1363,10 +1054,10 @@
     </row>
     <row r="21" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="14"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="10">
         <v>50000</v>
       </c>
@@ -1374,10 +1065,10 @@
     </row>
     <row r="22" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="11">
         <v>10</v>
       </c>
@@ -1385,10 +1076,10 @@
     </row>
     <row r="23" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="6">
         <f>IF(D20="","",1-(D21/D20)^(1/D22))</f>
         <v>0.20567176527571851</v>
@@ -1397,11 +1088,11 @@
     </row>
     <row r="24" spans="1:5" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1708,6 +1399,20 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
@@ -1716,20 +1421,6 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>